<commit_message>
Update position of Flash
</commit_message>
<xml_diff>
--- a/PCB_Rocket32_TRASIO_fixed/Rocket32_TRASIO_fixed_cpl1.xlsx
+++ b/PCB_Rocket32_TRASIO_fixed/Rocket32_TRASIO_fixed_cpl1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duy\PCB_Rocket32_TRASIO_fixed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617A4C9B-32FF-4937-B85A-CD098F6A701F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2269220D-F294-47C4-98A3-07A5F0A81A37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="50">
   <si>
     <t>Designator</t>
   </si>
@@ -136,6 +136,42 @@
   </si>
   <si>
     <t>Q8</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>100uF</t>
+  </si>
+  <si>
+    <t>LED-1206</t>
+  </si>
+  <si>
+    <t>TXB0108PWR</t>
+  </si>
+  <si>
+    <t>SOP65P640X120-20N</t>
+  </si>
+  <si>
+    <t>AMS1117-1.8</t>
+  </si>
+  <si>
+    <t>SOT229P700X180-4N</t>
+  </si>
+  <si>
+    <t>2N7002K-7</t>
+  </si>
+  <si>
+    <t>SOT96P240X100-3N</t>
+  </si>
+  <si>
+    <t>10k</t>
   </si>
 </sst>
 </file>
@@ -513,7 +549,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1782,7 +1818,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8DF2AA-D65F-4346-9D06-12C7C19C8B80}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D32"/>
@@ -1790,7 +1826,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1803,8 +1839,14 @@
       <c r="D1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1817,8 +1859,14 @@
       <c r="D2">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1831,8 +1879,14 @@
       <c r="D3">
         <v>270</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1845,8 +1899,14 @@
       <c r="D4">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1859,8 +1919,14 @@
       <c r="D5">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1873,8 +1939,14 @@
       <c r="D6">
         <v>270</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1887,8 +1959,14 @@
       <c r="D7">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1901,8 +1979,14 @@
       <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1915,8 +1999,14 @@
       <c r="D9">
         <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1929,8 +2019,14 @@
       <c r="D10">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1943,8 +2039,14 @@
       <c r="D11">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1957,8 +2059,14 @@
       <c r="D12">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1971,8 +2079,11 @@
       <c r="D13">
         <v>180</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1985,8 +2096,11 @@
       <c r="D14">
         <v>180</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1999,8 +2113,11 @@
       <c r="D15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2013,8 +2130,11 @@
       <c r="D16">
         <v>180</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2027,8 +2147,14 @@
       <c r="D17">
         <v>180</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2041,8 +2167,14 @@
       <c r="D18">
         <v>180</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -2055,8 +2187,14 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2069,8 +2207,14 @@
       <c r="D20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2083,8 +2227,14 @@
       <c r="D21">
         <v>270</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2097,8 +2247,14 @@
       <c r="D22">
         <v>270</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -2111,8 +2267,14 @@
       <c r="D23">
         <v>90</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -2125,8 +2287,14 @@
       <c r="D24">
         <v>270</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2139,8 +2307,14 @@
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2153,8 +2327,14 @@
       <c r="D26">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E26">
+        <v>330</v>
+      </c>
+      <c r="F26">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2167,8 +2347,14 @@
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -2181,8 +2367,14 @@
       <c r="D28">
         <v>90</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E28">
+        <v>330</v>
+      </c>
+      <c r="F28">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -2195,8 +2387,14 @@
       <c r="D29">
         <v>180</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -2209,8 +2407,14 @@
       <c r="D30">
         <v>270</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E30">
+        <v>330</v>
+      </c>
+      <c r="F30">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2223,8 +2427,14 @@
       <c r="D31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -2236,6 +2446,12 @@
       </c>
       <c r="D32">
         <v>90</v>
+      </c>
+      <c r="E32">
+        <v>330</v>
+      </c>
+      <c r="F32">
+        <v>1206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix SD card position
</commit_message>
<xml_diff>
--- a/PCB_Rocket32_TRASIO_fixed/Rocket32_TRASIO_fixed_cpl1.xlsx
+++ b/PCB_Rocket32_TRASIO_fixed/Rocket32_TRASIO_fixed_cpl1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duy\PCB_Rocket32_TRASIO_fixed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2269220D-F294-47C4-98A3-07A5F0A81A37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D4A038-7EB1-4B7F-90DB-3A2D989214A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Update position of SD card again
</commit_message>
<xml_diff>
--- a/PCB_Rocket32_TRASIO_fixed/Rocket32_TRASIO_fixed_cpl1.xlsx
+++ b/PCB_Rocket32_TRASIO_fixed/Rocket32_TRASIO_fixed_cpl1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duy\PCB_Rocket32_TRASIO_fixed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D4A038-7EB1-4B7F-90DB-3A2D989214A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B85142-07EE-4172-93BF-6FDEF5AD81EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
This should work man
</commit_message>
<xml_diff>
--- a/PCB_Rocket32_TRASIO_fixed/Rocket32_TRASIO_fixed_cpl1.xlsx
+++ b/PCB_Rocket32_TRASIO_fixed/Rocket32_TRASIO_fixed_cpl1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duy\PCB_Rocket32_TRASIO_fixed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B85142-07EE-4172-93BF-6FDEF5AD81EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD954A7B-2D61-4758-8D80-82175141BEF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -249,7 +249,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -269,6 +269,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -549,7 +552,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1124,11 +1127,11 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.15">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="4"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A35" s="4"/>
@@ -1820,7 +1823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8DF2AA-D65F-4346-9D06-12C7C19C8B80}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D32"/>
     </sheetView>
   </sheetViews>

</xml_diff>